<commit_message>
fixed missing ids for some datasets (fia, glonaf, climplant)
</commit_message>
<xml_diff>
--- a/ExternalDataSources.xlsx
+++ b/ExternalDataSources.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="423">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -920,6 +920,9 @@
     <t xml:space="preserve">Dubayah, R., J. B. Blair, S. Goetz, L. Fatoyinbo, M. Hansen, S. Healey, M. Hofton, G. Hurtt, J. Kellner, S. Luthcke, J. Armston, H. Tang, L. Duncanson, S. Hancock, P. Jantz, S. Marselis, P. L. Patterson, W. Qi, and C. Silva. 2020. The Global Ecosystem Dynamics Investigation: High-resolution laser ranging of the Earth’s forests and topography. Science of Remote Sensing 1:100002.</t>
   </si>
   <si>
+    <t xml:space="preserve">FIA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Forest Inventory and Analysis (FIA)</t>
   </si>
   <si>
@@ -1100,12 +1103,12 @@
     <t xml:space="preserve">phenocamr</t>
   </si>
   <si>
+    <t xml:space="preserve">ClimPlant</t>
+  </si>
+  <si>
     <t xml:space="preserve">BioclimaticDatabase</t>
   </si>
   <si>
-    <t xml:space="preserve">ClimPlant</t>
-  </si>
-  <si>
     <t xml:space="preserve">Realized climatic niches of vascular plants in European forest understoreys</t>
   </si>
   <si>
@@ -1899,6 +1902,9 @@
   </si>
   <si>
     <t xml:space="preserve">D. Ziolkowski, K. Pardieck, JR. Sauer. On the road again. For a bird survey that counts. Birding 42, 32-41 (2010)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GloNAF</t>
   </si>
   <si>
     <t xml:space="preserve">Global Naturalized Alien Flora</t>
@@ -2068,47 +2074,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2116,27 +2126,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2144,7 +2150,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2222,2508 +2228,2515 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="F35" activeCellId="0" sqref="F35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="G24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="39.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="43.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="2" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="24.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="3" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="4" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="35.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="60.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="43.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="82.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="25.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="39.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="234.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="24.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="4" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="14.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="35.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="60.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="43.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="82.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="L2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="12"/>
-      <c r="S2" s="0" t="s">
+      <c r="R2" s="13"/>
+      <c r="S2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="Q3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R3" s="12"/>
-      <c r="S3" s="0" t="s">
+      <c r="R3" s="13"/>
+      <c r="S3" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="12"/>
+      <c r="G4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q4" s="12" t="s">
+      <c r="Q4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="0" t="s">
+      <c r="R4" s="13"/>
+      <c r="S4" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="12"/>
+      <c r="G5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="12" t="s">
+      <c r="Q5" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="R5" s="12"/>
-      <c r="T5" s="12" t="s">
+      <c r="R5" s="13"/>
+      <c r="T5" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="U5" s="0" t="s">
+      <c r="U5" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="2" t="s">
+      <c r="H6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" s="3" t="s">
+      <c r="L6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="O6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Q6" s="12" t="s">
+      <c r="Q6" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="R6" s="12"/>
-      <c r="S6" s="0" t="s">
+      <c r="R6" s="13"/>
+      <c r="S6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T6" s="12" t="s">
+      <c r="T6" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="U6" s="0" t="s">
+      <c r="U6" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="3" t="s">
+      <c r="L7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="0" t="s">
+      <c r="O7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="0" t="s">
+      <c r="P7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q7" s="12" t="s">
+      <c r="Q7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="12"/>
-      <c r="S7" s="0" t="s">
+      <c r="R7" s="13"/>
+      <c r="S7" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="H8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M8" s="3" t="s">
+      <c r="L8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O8" s="0" t="s">
+      <c r="O8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="0" t="s">
+      <c r="P8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="Q8" s="12" t="s">
+      <c r="Q8" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="R8" s="12"/>
-      <c r="S8" s="0" t="s">
+      <c r="R8" s="13"/>
+      <c r="S8" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="L9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="Q9" s="12" t="s">
+      <c r="Q9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="R9" s="0" t="n">
+      <c r="R9" s="1" t="n">
         <v>2.05</v>
       </c>
-      <c r="S9" s="0" t="s">
+      <c r="S9" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="T9" s="0" t="s">
+      <c r="T9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="U9" s="0" t="s">
+      <c r="U9" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="H10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="L10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="O10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="Q10" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="S10" s="0" t="s">
+      <c r="S10" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="2" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="2" t="s">
+      <c r="H11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="3" t="s">
+      <c r="L11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="S11" s="0" t="s">
+      <c r="S11" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="2" t="s">
+      <c r="F12" s="12"/>
+      <c r="G12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="2" t="s">
+      <c r="H12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q12" s="0" t="s">
+      <c r="L12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="V12" s="0" t="s">
+      <c r="V12" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="2" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="2" t="s">
+      <c r="H13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q13" s="0" t="s">
+      <c r="L13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="V13" s="0" t="s">
+      <c r="V13" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="12"/>
+      <c r="G14" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="H14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q14" s="0" t="s">
+      <c r="L14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="2" t="s">
+      <c r="F15" s="17"/>
+      <c r="G15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="2" t="s">
+      <c r="H15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="L15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M15" s="3" t="s">
+      <c r="L15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="Q15" s="0" t="s">
+      <c r="Q15" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="12"/>
+      <c r="G16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="2" t="s">
+      <c r="H16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q16" s="12" t="s">
+      <c r="L16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q16" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="R16" s="12"/>
-      <c r="T16" s="12" t="s">
+      <c r="R16" s="13"/>
+      <c r="T16" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="U16" s="0" t="s">
+      <c r="U16" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="V16" s="12" t="s">
+      <c r="V16" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="2" t="s">
+      <c r="F17" s="12"/>
+      <c r="G17" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="2" t="s">
+      <c r="H17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="L17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M17" s="3" t="s">
+      <c r="L17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="12" t="s">
+      <c r="Q17" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="R17" s="12"/>
-      <c r="T17" s="12" t="s">
+      <c r="R17" s="13"/>
+      <c r="T17" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="U17" s="0" t="s">
+      <c r="U17" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="V17" s="12"/>
+      <c r="V17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="2" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="H18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M18" s="3" t="s">
+      <c r="L18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="O18" s="0" t="s">
+      <c r="O18" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Q18" s="12" t="s">
+      <c r="Q18" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="R18" s="12"/>
-      <c r="S18" s="0" t="s">
+      <c r="R18" s="13"/>
+      <c r="S18" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="T18" s="12" t="s">
+      <c r="T18" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="U18" s="0" t="s">
+      <c r="U18" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="V18" s="12"/>
+      <c r="V18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="2" t="s">
+      <c r="F19" s="12"/>
+      <c r="G19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I19" s="2" t="s">
+      <c r="H19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q19" s="12" t="s">
+      <c r="L19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="R19" s="12"/>
+      <c r="R19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="2" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="H20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="L20" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q20" s="12" t="s">
+      <c r="Q20" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="R20" s="12"/>
-      <c r="U20" s="0" t="s">
+      <c r="R20" s="13"/>
+      <c r="U20" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="2" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="H21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L21" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q21" s="12" t="s">
+      <c r="Q21" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="R21" s="12"/>
+      <c r="R21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="2" t="s">
+      <c r="F22" s="12"/>
+      <c r="G22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="2" t="s">
+      <c r="H22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="L22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q22" s="12" t="s">
+      <c r="Q22" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="R22" s="12"/>
-      <c r="T22" s="0" t="s">
+      <c r="R22" s="13"/>
+      <c r="T22" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="U22" s="0" t="s">
+      <c r="U22" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="2" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="H23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="J23" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="R23" s="12"/>
-      <c r="T23" s="0" t="s">
+      <c r="R23" s="13"/>
+      <c r="T23" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="U23" s="0" t="s">
+      <c r="U23" s="1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="2" t="s">
+      <c r="F24" s="12"/>
+      <c r="G24" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="H24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="L24" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M24" s="3" t="s">
+      <c r="L24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="Q24" s="12" t="s">
+      <c r="Q24" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="R24" s="12"/>
-      <c r="S24" s="0" t="s">
+      <c r="R24" s="13"/>
+      <c r="S24" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="T24" s="12" t="s">
+      <c r="T24" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="U24" s="12"/>
-      <c r="V24" s="0" t="s">
+      <c r="U24" s="13"/>
+      <c r="V24" s="1" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="2" t="s">
+      <c r="F25" s="12"/>
+      <c r="G25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="H25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q25" s="12" t="s">
+      <c r="L25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="R25" s="12"/>
-      <c r="S25" s="0" t="s">
+      <c r="R25" s="13"/>
+      <c r="S25" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="T25" s="12"/>
-      <c r="U25" s="12"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="2" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="L26" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N26" s="4" t="s">
+      <c r="N26" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="Q26" s="12" t="s">
+      <c r="Q26" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="R26" s="12"/>
-      <c r="T26" s="12" t="s">
+      <c r="R26" s="13"/>
+      <c r="T26" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="U26" s="12"/>
+      <c r="U26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="2" t="s">
+      <c r="F27" s="12"/>
+      <c r="G27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="L27" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q27" s="12" t="s">
+      <c r="Q27" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="R27" s="12"/>
-      <c r="T27" s="12" t="s">
+      <c r="R27" s="13"/>
+      <c r="T27" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="U27" s="12"/>
+      <c r="U27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="2" t="s">
+      <c r="F28" s="12"/>
+      <c r="G28" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N28" s="4" t="s">
+      <c r="N28" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="Q28" s="12" t="s">
+      <c r="Q28" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="R28" s="12"/>
-      <c r="T28" s="12"/>
-      <c r="U28" s="0" t="s">
+      <c r="R28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="1" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="2" t="s">
+      <c r="F29" s="12"/>
+      <c r="G29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="2" t="s">
+      <c r="H29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="J29" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N29" s="4" t="s">
+      <c r="N29" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="Q29" s="12" t="s">
+      <c r="Q29" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="R29" s="12"/>
-      <c r="S29" s="0" t="s">
+      <c r="R29" s="13"/>
+      <c r="S29" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="T29" s="12"/>
-      <c r="U29" s="12"/>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="2" t="s">
+      <c r="F30" s="12"/>
+      <c r="G30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="2" t="s">
+      <c r="H30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="K30" s="3" t="s">
+      <c r="K30" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q30" s="12" t="s">
+      <c r="Q30" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="R30" s="12"/>
-      <c r="S30" s="0" t="s">
+      <c r="R30" s="13"/>
+      <c r="S30" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="T30" s="12" t="s">
+      <c r="T30" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="U30" s="0" t="s">
+      <c r="U30" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="2" t="s">
+      <c r="F31" s="12"/>
+      <c r="G31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I31" s="2" t="s">
+      <c r="H31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q31" s="12" t="s">
+      <c r="L31" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q31" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="R31" s="12"/>
-      <c r="T31" s="12" t="s">
+      <c r="R31" s="13"/>
+      <c r="T31" s="13" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="2" t="s">
+      <c r="F32" s="12"/>
+      <c r="G32" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="H32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q32" s="12" t="s">
+      <c r="Q32" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="R32" s="12"/>
-      <c r="T32" s="12"/>
+      <c r="R32" s="13"/>
+      <c r="T32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="H33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K33" s="3" t="s">
+      <c r="K33" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="L33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="3" t="s">
+      <c r="L33" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="Q33" s="12" t="s">
+      <c r="Q33" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="R33" s="12"/>
-      <c r="S33" s="0" t="s">
+      <c r="R33" s="13"/>
+      <c r="S33" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="T33" s="12"/>
-      <c r="V33" s="0" t="s">
+      <c r="T33" s="13"/>
+      <c r="V33" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="F34" s="13" t="n">
+      <c r="F34" s="14" t="n">
         <v>44779</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="H34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="J34" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="L34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q34" s="12" t="s">
+      <c r="L34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q34" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="R34" s="12"/>
-      <c r="S34" s="0" t="s">
+      <c r="R34" s="13"/>
+      <c r="S34" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="T34" s="17" t="s">
+      <c r="T34" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="U34" s="0" t="s">
+      <c r="U34" s="1" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="1" t="s">
+      <c r="A35" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="D35" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="E35" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="H35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="2" t="s">
+      <c r="G35" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J35" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="K35" s="3" t="s">
+      <c r="J35" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="L35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="3" t="s">
+      <c r="K35" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="N35" s="4" t="s">
+      <c r="L35" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="N35" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="O35" s="0" t="s">
+      <c r="O35" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Q35" s="12" t="s">
-        <v>258</v>
-      </c>
-      <c r="R35" s="12"/>
-      <c r="S35" s="0" t="s">
+      <c r="Q35" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="T35" s="17"/>
-      <c r="U35" s="0" t="s">
+      <c r="R35" s="13"/>
+      <c r="S35" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="V35" s="0" t="s">
+      <c r="T35" s="13"/>
+      <c r="U35" s="1" t="s">
         <v>261</v>
       </c>
+      <c r="V35" s="1" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="B36" s="1" t="s">
+      <c r="A36" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="2" t="s">
+      <c r="E36" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="2" t="s">
+      <c r="H36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M36" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="P36" s="0" t="s">
+      <c r="L36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="P36" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="Q36" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="R36" s="12"/>
-      <c r="S36" s="0" t="s">
+      <c r="Q36" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="T36" s="12" t="s">
+      <c r="R36" s="13"/>
+      <c r="S36" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="U36" s="0" t="s">
+      <c r="T36" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="V36" s="0" t="s">
+      <c r="U36" s="1" t="s">
         <v>270</v>
       </c>
+      <c r="V36" s="1" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="A37" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D37" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F37" s="11"/>
-      <c r="G37" s="2" t="s">
+      <c r="E37" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F37" s="12"/>
+      <c r="G37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="2" t="s">
+      <c r="H37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="L37" s="3" t="s">
+      <c r="J37" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="L37" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q37" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="R37" s="12"/>
-      <c r="T37" s="12"/>
+      <c r="Q37" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="R37" s="13"/>
+      <c r="T37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="A38" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F38" s="11"/>
-      <c r="G38" s="2" t="s">
+      <c r="E38" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F38" s="12"/>
+      <c r="G38" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="2" t="s">
+      <c r="H38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="3" t="s">
+      <c r="K38" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M38" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="N38" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="Q38" s="12" t="s">
+      <c r="N38" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="R38" s="12"/>
-      <c r="S38" s="0" t="s">
+      <c r="Q38" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="T38" s="17" t="s">
+      <c r="R38" s="13"/>
+      <c r="S38" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="U38" s="0" t="s">
+      <c r="T38" s="13" t="s">
         <v>285</v>
       </c>
+      <c r="U38" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="V38" s="18" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="1" t="s">
+      <c r="A39" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C39" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="F39" s="11" t="s">
+      <c r="E39" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="F39" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="2" t="s">
+      <c r="H39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="K39" s="3" t="s">
+      <c r="J39" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="L39" s="3" t="s">
+      <c r="K39" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="L39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N39" s="4" t="s">
+      <c r="N39" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="O39" s="0" t="s">
+      <c r="O39" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="Q39" s="12" t="s">
-        <v>293</v>
+      <c r="Q39" s="13" t="s">
+        <v>294</v>
       </c>
       <c r="R39" s="19" t="n">
         <v>1.2</v>
       </c>
-      <c r="T39" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="U39" s="0" t="s">
+      <c r="T39" s="13" t="s">
         <v>295</v>
       </c>
+      <c r="U39" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="V39" s="18"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F40" s="11"/>
-      <c r="G40" s="2" t="s">
+      <c r="E40" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="F40" s="12"/>
+      <c r="G40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="2" t="s">
+      <c r="H40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q40" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="R40" s="12"/>
-      <c r="T40" s="12" t="s">
+      <c r="Q40" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="U40" s="0" t="s">
+      <c r="R40" s="13"/>
+      <c r="T40" s="13" t="s">
         <v>303</v>
       </c>
+      <c r="U40" s="1" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="A41" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="B41" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="D41" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="F41" s="11"/>
-      <c r="G41" s="2" t="s">
+      <c r="E41" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="G41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="2" t="s">
+      <c r="H41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L41" s="3" t="s">
+      <c r="L41" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q41" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="R41" s="12"/>
+      <c r="Q41" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="R41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="A42" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F42" s="11"/>
-      <c r="G42" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="G42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I42" s="2" t="s">
+      <c r="H42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J42" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="L42" s="3" t="s">
+      <c r="J42" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="L42" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q42" s="12" t="s">
-        <v>312</v>
-      </c>
-      <c r="R42" s="12"/>
-      <c r="V42" s="0" t="s">
+      <c r="Q42" s="13" t="s">
         <v>313</v>
       </c>
+      <c r="R42" s="13"/>
+      <c r="V42" s="1" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="A43" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F43" s="11"/>
-      <c r="G43" s="2" t="s">
+      <c r="B43" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="2" t="s">
+      <c r="H43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J43" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="L43" s="3" t="s">
+      <c r="J43" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="L43" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q43" s="12" t="s">
+      <c r="Q43" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="R43" s="13"/>
+      <c r="S43" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="T43" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F44" s="12"/>
+      <c r="G44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J44" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="R43" s="12"/>
-      <c r="S43" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="T43" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="U43" s="0" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="2" t="s">
+      <c r="L44" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q44" s="13" t="s">
+        <v>324</v>
+      </c>
+      <c r="R44" s="13"/>
+      <c r="S44" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="T44" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="U44" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F45" s="12"/>
+      <c r="G45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H44" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I44" s="2" t="s">
+      <c r="H45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="L44" s="3" t="s">
+      <c r="J45" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L45" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q44" s="12" t="s">
-        <v>323</v>
-      </c>
-      <c r="R44" s="12"/>
-      <c r="S44" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="T44" s="12" t="s">
-        <v>325</v>
-      </c>
-      <c r="U44" s="0" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="F45" s="11"/>
-      <c r="G45" s="2" t="s">
+      <c r="Q45" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="R45" s="13"/>
+      <c r="U45" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F46" s="12"/>
+      <c r="G46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L45" s="3" t="s">
+      <c r="H46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L46" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q45" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="R45" s="12"/>
-      <c r="U45" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="V45" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F46" s="11"/>
-      <c r="G46" s="2" t="s">
+      <c r="Q46" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="R46" s="13"/>
+      <c r="S46" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="T46" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="U46" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I46" s="2" t="s">
+      <c r="H47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L46" s="3" t="s">
+      <c r="K47" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q47" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="S47" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="T47" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="U47" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="F48" s="12"/>
+      <c r="G48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L48" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q46" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="R46" s="12"/>
-      <c r="S46" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="T46" s="12" t="s">
-        <v>339</v>
-      </c>
-      <c r="U46" s="0" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="F47" s="11"/>
-      <c r="G47" s="2" t="s">
+      <c r="Q48" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="R48" s="13"/>
+      <c r="T48" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="U48" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="F49" s="12"/>
+      <c r="G49" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="2" t="s">
+      <c r="H49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="L49" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q49" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="R49" s="13"/>
+      <c r="S49" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="T49" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="U49" s="13"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>373</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K47" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q47" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="R47" s="0" t="s">
-        <v>348</v>
-      </c>
-      <c r="S47" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="T47" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="U47" s="0" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="F48" s="11"/>
-      <c r="G48" s="2" t="s">
+      <c r="K50" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q50" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="R50" s="13"/>
+      <c r="S50" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="T50" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="U50" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="V50" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F51" s="12"/>
+      <c r="G51" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H48" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="L48" s="3" t="s">
+      <c r="H51" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M51" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q51" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="R51" s="13"/>
+      <c r="S51" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="T51" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="F52" s="12"/>
+      <c r="G52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L52" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="Q48" s="12" t="s">
-        <v>357</v>
-      </c>
-      <c r="R48" s="12"/>
-      <c r="T48" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="U48" s="0" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="F49" s="11"/>
-      <c r="G49" s="2" t="s">
+      <c r="Q52" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="V52" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="F53" s="12"/>
+      <c r="G53" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q49" s="12" t="s">
-        <v>365</v>
-      </c>
-      <c r="R49" s="12"/>
-      <c r="S49" s="0" t="s">
-        <v>366</v>
-      </c>
-      <c r="T49" s="12" t="s">
-        <v>367</v>
-      </c>
-      <c r="U49" s="12"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
-        <v>368</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I50" s="2" t="s">
+      <c r="H53" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q50" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="R50" s="12"/>
-      <c r="S50" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="T50" s="17" t="s">
-        <v>376</v>
-      </c>
-      <c r="U50" s="0" t="s">
-        <v>377</v>
-      </c>
-      <c r="V50" s="0" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
-        <v>379</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C51" s="1" t="s">
+      <c r="L53" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q53" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="S53" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="U53" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="V53" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="F51" s="11"/>
-      <c r="G51" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I51" s="2" t="s">
+      <c r="C54" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="F54" s="12"/>
+      <c r="G54" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J51" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N51" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q51" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="R51" s="12"/>
-      <c r="S51" s="0" t="s">
-        <v>218</v>
-      </c>
-      <c r="T51" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="U51" s="0" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>388</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="L54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="S54" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="T54" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="U54" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="F52" s="11"/>
-      <c r="G52" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q52" s="0" t="s">
-        <v>391</v>
-      </c>
-      <c r="V52" s="0" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>393</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="F53" s="11"/>
-      <c r="G53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="N53" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q53" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="S53" s="0" t="s">
-        <v>398</v>
-      </c>
-      <c r="T53" s="12" t="s">
-        <v>399</v>
-      </c>
-      <c r="U53" s="0" t="s">
-        <v>400</v>
-      </c>
-      <c r="V53" s="0" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>402</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="F54" s="11"/>
-      <c r="G54" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q54" s="0" t="s">
-        <v>407</v>
-      </c>
-      <c r="S54" s="0" t="s">
-        <v>408</v>
-      </c>
-      <c r="T54" s="0" t="s">
-        <v>409</v>
-      </c>
-      <c r="U54" s="0" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>412</v>
+      <c r="D55" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>414</v>
       </c>
       <c r="F55" s="20" t="n">
         <v>45235</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="G55" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H55" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="2" t="s">
+      <c r="H55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L55" s="3" t="s">
+      <c r="L55" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N55" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q55" s="0" t="s">
-        <v>413</v>
-      </c>
-      <c r="S55" s="0" t="s">
-        <v>414</v>
-      </c>
-      <c r="T55" s="0" t="s">
+      <c r="N55" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q55" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="U55" s="0" t="s">
+      <c r="S55" s="1" t="s">
         <v>416</v>
+      </c>
+      <c r="T55" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="U55" s="1" t="s">
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -4798,7 +4811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4808,22 +4821,22 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>417</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>418</v>
+      <c r="A2" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>419</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>420</v>
+      <c r="A3" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Root system of Individual Plants
</commit_message>
<xml_diff>
--- a/ExternalDataSources.xlsx
+++ b/ExternalDataSources.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="431">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -732,6 +732,30 @@
   </si>
   <si>
     <t xml:space="preserve">Choat B., Jansen S., Brodribb T.J., Cochard H., Delzon S., Bhaskar R., Bucci S., Feild T.S., Gleason S.M., Hacke U.G., Jacobsen A.L., Lens F., Maherali H., Martinez-Vilalta J., Mayr S., Mencuccini M., Mitchell P.J., Nardini A., Pittermann J., Pratt R.B., Sperry J.S., Westoby M., Wright I.J., Zanne A. (2012) Global convergence in the vulnerability of forests to drought. Nature 491: 752-755.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root systems of individual plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains 5,647 observations, to our knowledge the largest database describing the maximum rooting depth, lateral spread, and shoot size of terrestrial plants in the world</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XLSX, CSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pasta.lternet.edu/package/metadata/eml/knb-lter-hfr/426/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rooting depth and spread, shoot height and width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1111/nph.18031</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tumber-Dávila, Shersingh Joseph and Schenk, H. Jochen and Du, Enzai and Jackson, Robert B. New Phytologist (2022) 235: 1032–1056</t>
   </si>
   <si>
     <t xml:space="preserve">sPlot</t>
@@ -1945,7 +1969,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1991,6 +2015,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2069,7 +2100,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2142,16 +2173,20 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2228,19 +2263,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="G24" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="G11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="25.28"/>
@@ -3511,18 +3546,20 @@
         <v>213</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="12"/>
+      <c r="F29" s="18" t="n">
+        <v>45118</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>51</v>
       </c>
@@ -3532,40 +3569,45 @@
       <c r="I29" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J29" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="L29" s="4" t="s">
         <v>84</v>
       </c>
       <c r="N29" s="5" t="s">
         <v>200</v>
       </c>
+      <c r="O29" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="Q29" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="R29" s="13"/>
+      <c r="R29" s="19"/>
       <c r="S29" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="T29" s="13"/>
-      <c r="U29" s="13"/>
+      <c r="T29" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="V29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="3" t="s">
@@ -3578,43 +3620,39 @@
         <v>107</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="N30" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="Q30" s="13" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R30" s="13"/>
       <c r="S30" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="T30" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="U30" s="1" t="s">
-        <v>224</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F31" s="12"/>
       <c r="G31" s="3" t="s">
@@ -3626,32 +3664,44 @@
       <c r="I31" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="J31" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="L31" s="4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="Q31" s="13" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="R31" s="13"/>
+      <c r="S31" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="T31" s="13" t="s">
-        <v>229</v>
+        <v>231</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="3" t="s">
@@ -3664,33 +3714,35 @@
         <v>107</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="Q32" s="13" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="R32" s="13"/>
-      <c r="T32" s="13"/>
+      <c r="T32" s="13" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F33" s="12"/>
       <c r="G33" s="3" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>28</v>
@@ -3698,72 +3750,59 @@
       <c r="I33" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K33" s="4" t="s">
-        <v>239</v>
-      </c>
       <c r="L33" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="4" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
       <c r="Q33" s="13" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="R33" s="13"/>
-      <c r="S33" s="1" t="s">
-        <v>241</v>
-      </c>
       <c r="T33" s="13"/>
-      <c r="V33" s="1" t="s">
-        <v>242</v>
-      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F34" s="14" t="n">
-        <v>44779</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="F34" s="12"/>
       <c r="G34" s="3" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>246</v>
+        <v>107</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="M34" s="4" t="s">
+        <v>224</v>
+      </c>
       <c r="Q34" s="13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="R34" s="13"/>
       <c r="S34" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="T34" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="U34" s="1" t="s">
+      <c r="T34" s="13"/>
+      <c r="V34" s="1" t="s">
         <v>250</v>
       </c>
     </row>
@@ -3775,7 +3814,7 @@
         <v>180</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>252</v>
@@ -3783,11 +3822,11 @@
       <c r="E35" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="F35" s="14" t="s">
-        <v>254</v>
+      <c r="F35" s="14" t="n">
+        <v>44779</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>255</v>
+        <v>51</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>28</v>
@@ -3796,63 +3835,58 @@
         <v>29</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M35" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="Q35" s="13" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="R35" s="13"/>
       <c r="S35" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="T35" s="13"/>
+        <v>256</v>
+      </c>
+      <c r="T35" s="13" t="s">
+        <v>257</v>
+      </c>
       <c r="U35" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="V35" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="H36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E36" s="2" t="s">
+      <c r="K36" s="4" t="s">
         <v>265</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>28</v>
@@ -3860,8 +3894,11 @@
       <c r="M36" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="P36" s="1" t="s">
-        <v>101</v>
+      <c r="N36" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="Q36" s="13" t="s">
         <v>267</v>
@@ -3870,31 +3907,29 @@
       <c r="S36" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="T36" s="13" t="s">
+      <c r="T36" s="13"/>
+      <c r="U36" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="U36" s="1" t="s">
+      <c r="V36" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="V36" s="1" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="3" t="s">
@@ -3904,35 +3939,49 @@
         <v>28</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J37" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q37" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="L37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q37" s="13" t="s">
+      <c r="R37" s="13"/>
+      <c r="S37" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="R37" s="13"/>
-      <c r="T37" s="13"/>
+      <c r="T37" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="F38" s="12"/>
       <c r="G38" s="3" t="s">
@@ -3942,149 +3991,147 @@
         <v>28</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>281</v>
+        <v>29</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N38" s="5" t="s">
-        <v>282</v>
+        <v>84</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="R38" s="13"/>
-      <c r="S38" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="T38" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="U38" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="V38" s="18" t="s">
-        <v>287</v>
-      </c>
+      <c r="T38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="F39" s="12"/>
+      <c r="G39" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="L39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N39" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="Q39" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J39" s="3" t="s">
+      <c r="R39" s="13"/>
+      <c r="S39" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="T39" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="L39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="N39" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q39" s="13" t="s">
+      <c r="U39" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="R39" s="19" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="T39" s="13" t="s">
+      <c r="V39" s="21" t="s">
         <v>295</v>
       </c>
-      <c r="U39" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="V39" s="18"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="F40" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="G40" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="K40" s="4" t="s">
         <v>301</v>
-      </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="N40" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="Q40" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="R40" s="13"/>
+      <c r="R40" s="19" t="n">
+        <v>1.2</v>
+      </c>
       <c r="T40" s="13" t="s">
         <v>303</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>304</v>
       </c>
+      <c r="V40" s="21"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F41" s="12"/>
       <c r="G41" s="3" t="s">
@@ -4094,31 +4141,37 @@
         <v>28</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q41" s="13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="R41" s="13"/>
+      <c r="T41" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="F42" s="12"/>
       <c r="G42" s="3" t="s">
@@ -4130,35 +4183,29 @@
       <c r="I42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J42" s="3" t="s">
-        <v>312</v>
-      </c>
       <c r="L42" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q42" s="13" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="R42" s="13"/>
-      <c r="V42" s="1" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F43" s="12"/>
       <c r="G43" s="3" t="s">
@@ -4171,37 +4218,34 @@
         <v>29</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="L43" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q43" s="13" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="R43" s="13"/>
-      <c r="S43" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="T43" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="U43" s="1" t="s">
-        <v>321</v>
+      <c r="V43" s="1" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>323</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>324</v>
       </c>
       <c r="F44" s="12"/>
       <c r="G44" s="3" t="s">
@@ -4214,40 +4258,37 @@
         <v>29</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q44" s="13" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="R44" s="13"/>
       <c r="S44" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="T44" s="13" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="U44" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="3" t="s">
@@ -4260,37 +4301,40 @@
         <v>29</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>52</v>
+        <v>325</v>
       </c>
       <c r="L45" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q45" s="13" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="R45" s="13"/>
+      <c r="S45" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="T45" s="13" t="s">
+        <v>334</v>
+      </c>
       <c r="U45" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="V45" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>336</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="3" t="s">
@@ -4300,22 +4344,22 @@
         <v>28</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>107</v>
+        <v>29</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="L46" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q46" s="13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="R46" s="13"/>
-      <c r="S46" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="T46" s="13" t="s">
+      <c r="U46" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="U46" s="1" t="s">
+      <c r="V46" s="1" t="s">
         <v>341</v>
       </c>
     </row>
@@ -4324,7 +4368,7 @@
         <v>342</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>343</v>
@@ -4345,46 +4389,38 @@
       <c r="I47" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="L47" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q47" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="L47" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M47" s="4" t="s">
+      <c r="R47" s="13"/>
+      <c r="S47" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="Q47" s="13" t="s">
+      <c r="T47" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="R47" s="1" t="s">
+      <c r="U47" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="S47" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="T47" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>357</v>
       </c>
       <c r="F48" s="12"/>
       <c r="G48" s="3" t="s">
@@ -4394,15 +4430,26 @@
         <v>28</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>157</v>
+        <v>107</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>354</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>84</v>
+        <v>28</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="Q48" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="S48" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="R48" s="13"/>
       <c r="T48" s="13" t="s">
         <v>359</v>
       </c>
@@ -4415,16 +4462,16 @@
         <v>361</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F49" s="12"/>
       <c r="G49" s="3" t="s">
@@ -4436,9 +4483,6 @@
       <c r="I49" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J49" s="3" t="s">
-        <v>365</v>
-      </c>
       <c r="L49" s="4" t="s">
         <v>84</v>
       </c>
@@ -4446,20 +4490,19 @@
         <v>366</v>
       </c>
       <c r="R49" s="13"/>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="13" t="s">
         <v>367</v>
       </c>
-      <c r="T49" s="13" t="s">
+      <c r="U49" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="U49" s="13"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>369</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>370</v>
@@ -4470,9 +4513,7 @@
       <c r="E50" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="F50" s="12" t="s">
-        <v>373</v>
-      </c>
+      <c r="F50" s="12"/>
       <c r="G50" s="3" t="s">
         <v>51</v>
       </c>
@@ -4480,48 +4521,45 @@
         <v>28</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K50" s="4" t="s">
-        <v>374</v>
+        <v>157</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>373</v>
       </c>
       <c r="L50" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q50" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="R50" s="13"/>
       <c r="S50" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="T50" s="13" t="s">
         <v>376</v>
       </c>
-      <c r="T50" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="U50" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="V50" s="1" t="s">
-        <v>379</v>
-      </c>
+      <c r="U50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="F51" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="F51" s="12"/>
       <c r="G51" s="3" t="s">
         <v>51</v>
       </c>
@@ -4531,47 +4569,41 @@
       <c r="I51" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J51" s="3" t="s">
-        <v>216</v>
-      </c>
       <c r="K51" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M51" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="N51" s="5" t="s">
-        <v>385</v>
+        <v>84</v>
       </c>
       <c r="Q51" s="13" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="R51" s="13"/>
       <c r="S51" s="1" t="s">
-        <v>218</v>
+        <v>384</v>
       </c>
       <c r="T51" s="13" t="s">
+        <v>385</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="V51" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="U51" s="1" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>390</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>391</v>
@@ -4586,31 +4618,50 @@
       <c r="I52" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="J52" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>392</v>
+      </c>
       <c r="L52" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="V52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="N52" s="5" t="s">
         <v>393</v>
+      </c>
+      <c r="Q52" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="R52" s="13"/>
+      <c r="S52" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="T52" s="13" t="s">
+        <v>395</v>
+      </c>
+      <c r="U52" s="1" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>381</v>
+        <v>389</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="F53" s="12"/>
       <c r="G53" s="3" t="s">
@@ -4623,49 +4674,34 @@
         <v>107</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="N53" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q53" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="S53" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="T53" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q53" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="U53" s="1" t="s">
+      <c r="V53" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="V53" s="1" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="F54" s="12"/>
       <c r="G54" s="3" t="s">
-        <v>407</v>
+        <v>51</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>28</v>
@@ -4677,30 +4713,36 @@
         <v>28</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q54" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q54" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="S54" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="T54" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="V54" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>390</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>413</v>
@@ -4708,37 +4750,83 @@
       <c r="E55" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="F55" s="20" t="n">
+      <c r="F55" s="12"/>
+      <c r="G55" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="T55" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="U55" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="F56" s="18" t="n">
         <v>45235</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H55" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I55" s="3" t="s">
+      <c r="H56" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="L56" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="N55" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="Q55" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="S55" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="T55" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="U55" s="1" t="s">
-        <v>418</v>
-      </c>
-    </row>
+      <c r="N56" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="U56" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" display="https://cds.climate.copernicus.eu"/>
@@ -4767,38 +4855,40 @@
     <hyperlink ref="Q27" r:id="rId24" display="https://roots.ornl.gov/"/>
     <hyperlink ref="T27" r:id="rId25" display="https://doi.org/10.1111/nph.14486"/>
     <hyperlink ref="Q28" r:id="rId26" display="https://xylemfunctionaltraits.org/"/>
-    <hyperlink ref="Q29" r:id="rId27" display="https://www.idiv.de/de/splot.html"/>
-    <hyperlink ref="Q30" r:id="rId28" display="https://doi.org/10.25829/idiv.3474-40-3292"/>
-    <hyperlink ref="T30" r:id="rId29" display="https://doi.org/10.1111/geb.13346"/>
-    <hyperlink ref="Q31" r:id="rId30" display="https://lotvs.csic.es/"/>
-    <hyperlink ref="T31" r:id="rId31" display="https://www.biorxiv.org/content/10.1101/2021.09.29.462383v1.full"/>
-    <hyperlink ref="Q32" r:id="rId32" display="https://gfbinitiative.net/"/>
-    <hyperlink ref="Q33" r:id="rId33" display="http://icp-forests.net/"/>
-    <hyperlink ref="T34" r:id="rId34" display="https://doi.org/10.1016/j.srs.2020.100002"/>
-    <hyperlink ref="Q36" r:id="rId35" display="http://sapfluxnet.creaf.cat/"/>
-    <hyperlink ref="T36" r:id="rId36" display="https://doi.org/10.5194/essd-13-2607-2021"/>
-    <hyperlink ref="Q40" r:id="rId37" location="/home" display="https://data.isric.org/geonetwork/srv/eng/catalog.search#/home"/>
-    <hyperlink ref="T40" r:id="rId38" display="https://doi.org/10.5194/essd-9-1-2017"/>
-    <hyperlink ref="Q41" r:id="rId39" display="https://www.fao.org/soils-portal/data-hub/soil-maps-and-databases/harmonized-world-soil-database-v12/en/"/>
-    <hyperlink ref="Q42" r:id="rId40" display="https://soilgrids.org/"/>
-    <hyperlink ref="Q43" r:id="rId41" display="https://www.isric.org/explore/wise-databases"/>
-    <hyperlink ref="T43" r:id="rId42" display="https://doi.org/10.1016/j.geoderma.2016.01.034"/>
-    <hyperlink ref="Q44" r:id="rId43" display="http://globalchange.bnu.edu.cn/research/data"/>
-    <hyperlink ref="T44" r:id="rId44" display="http://doi.wiley.com/10.1002/2013MS000293"/>
-    <hyperlink ref="Q45" r:id="rId45" display="https://www.futurewater.eu/projects/hihydrosoil/"/>
-    <hyperlink ref="Q46" r:id="rId46" display="https://ismn.earth/en/"/>
-    <hyperlink ref="T46" r:id="rId47" display="https://doi.org/10.5194/hess-2021-2"/>
-    <hyperlink ref="Q47" r:id="rId48" display="https://doi.org/10.3334/ORNLDAAC/1827"/>
-    <hyperlink ref="T47" r:id="rId49" display="https://10.5194/bg-7-1915-2010"/>
-    <hyperlink ref="Q48" r:id="rId50" display="https://doi.pangaea.de/10.1594/PANGAEA.788537"/>
-    <hyperlink ref="T48" r:id="rId51" display="https://doi.org/10.1029/2012GC004370"/>
-    <hyperlink ref="Q49" r:id="rId52" display="https://dataverse.scholarsportal.info/dataset.xhtml"/>
-    <hyperlink ref="T49" r:id="rId53" display="https://doi.org/10.1002/2017GL075860"/>
-    <hyperlink ref="T50" r:id="rId54" display="https://doi.org/10.1016/j.cageo.2014.07.020"/>
-    <hyperlink ref="Q51" r:id="rId55" display="https://biotime.st-andrews.ac.uk/"/>
-    <hyperlink ref="T51" r:id="rId56" display="https://doi.org/10.1111/geb.12729"/>
-    <hyperlink ref="Q53" r:id="rId57" display="https://compadre-db.org/"/>
-    <hyperlink ref="T53" r:id="rId58" display="https://doi.org/10.1111/1365-2745.12334"/>
+    <hyperlink ref="Q29" r:id="rId27" display="https://pasta.lternet.edu/package/metadata/eml/knb-lter-hfr/426/1"/>
+    <hyperlink ref="T29" r:id="rId28" display="https://doi.org/10.1111/nph.18031"/>
+    <hyperlink ref="Q30" r:id="rId29" display="https://www.idiv.de/de/splot.html"/>
+    <hyperlink ref="Q31" r:id="rId30" display="https://doi.org/10.25829/idiv.3474-40-3292"/>
+    <hyperlink ref="T31" r:id="rId31" display="https://doi.org/10.1111/geb.13346"/>
+    <hyperlink ref="Q32" r:id="rId32" display="https://lotvs.csic.es/"/>
+    <hyperlink ref="T32" r:id="rId33" display="https://www.biorxiv.org/content/10.1101/2021.09.29.462383v1.full"/>
+    <hyperlink ref="Q33" r:id="rId34" display="https://gfbinitiative.net/"/>
+    <hyperlink ref="Q34" r:id="rId35" display="http://icp-forests.net/"/>
+    <hyperlink ref="T35" r:id="rId36" display="https://doi.org/10.1016/j.srs.2020.100002"/>
+    <hyperlink ref="Q37" r:id="rId37" display="http://sapfluxnet.creaf.cat/"/>
+    <hyperlink ref="T37" r:id="rId38" display="https://doi.org/10.5194/essd-13-2607-2021"/>
+    <hyperlink ref="Q41" r:id="rId39" location="/home" display="https://data.isric.org/geonetwork/srv/eng/catalog.search#/home"/>
+    <hyperlink ref="T41" r:id="rId40" display="https://doi.org/10.5194/essd-9-1-2017"/>
+    <hyperlink ref="Q42" r:id="rId41" display="https://www.fao.org/soils-portal/data-hub/soil-maps-and-databases/harmonized-world-soil-database-v12/en/"/>
+    <hyperlink ref="Q43" r:id="rId42" display="https://soilgrids.org/"/>
+    <hyperlink ref="Q44" r:id="rId43" display="https://www.isric.org/explore/wise-databases"/>
+    <hyperlink ref="T44" r:id="rId44" display="https://doi.org/10.1016/j.geoderma.2016.01.034"/>
+    <hyperlink ref="Q45" r:id="rId45" display="http://globalchange.bnu.edu.cn/research/data"/>
+    <hyperlink ref="T45" r:id="rId46" display="http://doi.wiley.com/10.1002/2013MS000293"/>
+    <hyperlink ref="Q46" r:id="rId47" display="https://www.futurewater.eu/projects/hihydrosoil/"/>
+    <hyperlink ref="Q47" r:id="rId48" display="https://ismn.earth/en/"/>
+    <hyperlink ref="T47" r:id="rId49" display="https://doi.org/10.5194/hess-2021-2"/>
+    <hyperlink ref="Q48" r:id="rId50" display="https://doi.org/10.3334/ORNLDAAC/1827"/>
+    <hyperlink ref="T48" r:id="rId51" display="https://10.5194/bg-7-1915-2010"/>
+    <hyperlink ref="Q49" r:id="rId52" display="https://doi.pangaea.de/10.1594/PANGAEA.788537"/>
+    <hyperlink ref="T49" r:id="rId53" display="https://doi.org/10.1029/2012GC004370"/>
+    <hyperlink ref="Q50" r:id="rId54" display="https://dataverse.scholarsportal.info/dataset.xhtml"/>
+    <hyperlink ref="T50" r:id="rId55" display="https://doi.org/10.1002/2017GL075860"/>
+    <hyperlink ref="T51" r:id="rId56" display="https://doi.org/10.1016/j.cageo.2014.07.020"/>
+    <hyperlink ref="Q52" r:id="rId57" display="https://biotime.st-andrews.ac.uk/"/>
+    <hyperlink ref="T52" r:id="rId58" display="https://doi.org/10.1111/geb.12729"/>
+    <hyperlink ref="Q54" r:id="rId59" display="https://compadre-db.org/"/>
+    <hyperlink ref="T54" r:id="rId60" display="https://doi.org/10.1111/1365-2745.12334"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -4811,7 +4901,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -4821,22 +4911,22 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>420</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>422</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The china plant trait database
</commit_message>
<xml_diff>
--- a/ExternalDataSources.xlsx
+++ b/ExternalDataSources.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="492">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -894,6 +894,27 @@
   </si>
   <si>
     <t xml:space="preserve">Tavşanoglu, C., and J. G. Pausas. 2018. A functional trait database for Mediterranean Basin plants. Scientific Data 5:1–18.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPTD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The China plant trait database version 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China Plant Trait Database contains information on morphometric, physical, chemical, photosynthetic and hydraulic traits from 1529 unique species in 140 sites spanning a diversity of vegetation types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.6084/m9.figshare.19448219.v6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1038/s41597-022-01884-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wang, H., Harrison, S.P., Li, M. et al. The China plant trait database version 2. Sci Data 9, 769 (2022)</t>
   </si>
   <si>
     <t xml:space="preserve">sPlot</t>
@@ -2132,7 +2153,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2180,16 +2201,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2268,7 +2284,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2357,11 +2373,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2447,15 +2459,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V63"/>
+  <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="G2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="G11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="O37" activeCellId="0" sqref="O37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="25.28"/>
@@ -3943,7 +3955,7 @@
       <c r="C33" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="16" t="s">
         <v>247</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -3995,7 +4007,7 @@
       <c r="C34" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="16" t="s">
         <v>254</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -4032,7 +4044,7 @@
       <c r="T34" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="U34" s="23" t="s">
+      <c r="U34" s="22" t="s">
         <v>259</v>
       </c>
       <c r="V34" s="20"/>
@@ -4047,7 +4059,7 @@
       <c r="C35" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="16" t="s">
         <v>261</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -4081,30 +4093,32 @@
       <c r="T35" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="U35" s="23" t="s">
+      <c r="U35" s="22" t="s">
         <v>266</v>
       </c>
       <c r="V35" s="20"/>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>267</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="16" t="s">
         <v>268</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>267</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="F36" s="12"/>
+      <c r="F36" s="21" t="s">
+        <v>241</v>
+      </c>
       <c r="G36" s="3" t="s">
-        <v>51</v>
+        <v>270</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>28</v>
@@ -4112,40 +4126,47 @@
       <c r="I36" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J36" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="L36" s="4" t="s">
         <v>84</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>200</v>
       </c>
+      <c r="O36" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="Q36" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="R36" s="13"/>
+      <c r="R36" s="19" t="n">
+        <v>2</v>
+      </c>
       <c r="S36" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="T36" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
+      <c r="U36" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="V36" s="20"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F37" s="12"/>
       <c r="G37" s="3" t="s">
@@ -4158,37 +4179,33 @@
         <v>107</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="N37" s="5" t="s">
+        <v>200</v>
+      </c>
       <c r="Q37" s="13" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="R37" s="13"/>
       <c r="S37" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="T37" s="13" t="s">
-        <v>277</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>278</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>280</v>
@@ -4206,32 +4223,44 @@
       <c r="I38" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="J38" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>282</v>
+      </c>
       <c r="L38" s="4" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="Q38" s="13" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="R38" s="13"/>
+      <c r="S38" s="1" t="s">
+        <v>279</v>
+      </c>
       <c r="T38" s="13" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F39" s="12"/>
       <c r="G39" s="3" t="s">
@@ -4244,33 +4273,35 @@
         <v>107</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="Q39" s="13" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="R39" s="13"/>
-      <c r="T39" s="13"/>
+      <c r="T39" s="13" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="3" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>28</v>
@@ -4278,36 +4309,24 @@
       <c r="I40" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K40" s="4" t="s">
-        <v>293</v>
-      </c>
       <c r="L40" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
       <c r="Q40" s="13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="R40" s="13"/>
-      <c r="S40" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="T40" s="13"/>
-      <c r="V40" s="1" t="s">
-        <v>296</v>
-      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>298</v>
@@ -4315,23 +4334,24 @@
       <c r="E41" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F41" s="14" t="n">
-        <v>44779</v>
-      </c>
+      <c r="F41" s="12"/>
       <c r="G41" s="3" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="H41" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>300</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="Q41" s="13" t="s">
         <v>301</v>
@@ -4340,34 +4360,32 @@
       <c r="S41" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="T41" s="13" t="s">
+      <c r="T41" s="13"/>
+      <c r="V41" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="U41" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>308</v>
+      <c r="F42" s="14" t="n">
+        <v>44779</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>309</v>
+        <v>51</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>28</v>
@@ -4376,59 +4394,46 @@
         <v>29</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M42" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="Q42" s="13" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="R42" s="13"/>
       <c r="S42" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="T42" s="13"/>
+        <v>309</v>
+      </c>
+      <c r="T42" s="13" t="s">
+        <v>310</v>
+      </c>
       <c r="U42" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="V42" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D43" s="16" t="s">
-        <v>318</v>
+        <v>297</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>313</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>28</v>
@@ -4436,8 +4441,17 @@
       <c r="I43" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="J43" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>318</v>
+      </c>
       <c r="L43" s="4" t="s">
-        <v>84</v>
+        <v>28</v>
+      </c>
+      <c r="M43" s="4" t="s">
+        <v>319</v>
       </c>
       <c r="N43" s="5" t="s">
         <v>200</v>
@@ -4445,86 +4459,86 @@
       <c r="O43" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="P43" s="24" t="s">
-        <v>322</v>
-      </c>
       <c r="Q43" s="13" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="R43" s="13"/>
       <c r="S43" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="T43" s="13"/>
-      <c r="V43" s="1"/>
+      <c r="U43" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D44" s="16" t="s">
         <v>325</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="F44" s="12"/>
       <c r="G44" s="3" t="s">
-        <v>51</v>
+        <v>328</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>107</v>
+        <v>29</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M44" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>101</v>
+        <v>84</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="P44" s="23" t="s">
+        <v>329</v>
       </c>
       <c r="Q44" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="R44" s="13"/>
       <c r="S44" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="T44" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="U44" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="V44" s="1" t="s">
-        <v>333</v>
-      </c>
+      <c r="T44" s="13"/>
+      <c r="V44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>197</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="F45" s="12"/>
       <c r="G45" s="3" t="s">
@@ -4534,35 +4548,49 @@
         <v>28</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J45" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L45" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q45" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="R45" s="13"/>
+      <c r="S45" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="L45" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q45" s="13" t="s">
+      <c r="T45" s="13" t="s">
         <v>338</v>
       </c>
-      <c r="R45" s="13"/>
-      <c r="T45" s="13"/>
+      <c r="U45" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="V45" s="1" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>341</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="F46" s="12"/>
       <c r="G46" s="3" t="s">
@@ -4572,140 +4600,138 @@
         <v>28</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K46" s="4" t="s">
-        <v>343</v>
+        <v>29</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>344</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M46" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="N46" s="5" t="s">
-        <v>344</v>
+        <v>84</v>
       </c>
       <c r="Q46" s="13" t="s">
         <v>345</v>
       </c>
       <c r="R46" s="13"/>
-      <c r="S46" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="T46" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="U46" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="V46" s="20" t="s">
-        <v>349</v>
-      </c>
+      <c r="T46" s="13"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>180</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="F47" s="12"/>
+      <c r="G47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N47" s="5" t="s">
         <v>351</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="Q47" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="F47" s="12" t="s">
+      <c r="R47" s="13"/>
+      <c r="S47" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J47" s="3" t="s">
+      <c r="T47" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="K47" s="4" t="s">
+      <c r="U47" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="L47" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="N47" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q47" s="13" t="s">
+      <c r="V47" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="R47" s="19" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="T47" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="U47" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="V47" s="20"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="F48" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="G48" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J48" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="K48" s="4" t="s">
         <v>362</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="F48" s="12"/>
-      <c r="G48" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="L48" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="N48" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>147</v>
+      </c>
       <c r="Q48" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="R48" s="19" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="T48" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="R48" s="13"/>
-      <c r="T48" s="13" t="s">
+      <c r="U48" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="U48" s="1" t="s">
-        <v>366</v>
-      </c>
+      <c r="V48" s="20"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>368</v>
@@ -4724,7 +4750,7 @@
         <v>28</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="L49" s="4" t="s">
         <v>84</v>
@@ -4733,22 +4759,28 @@
         <v>371</v>
       </c>
       <c r="R49" s="13"/>
+      <c r="T49" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="F50" s="12"/>
       <c r="G50" s="3" t="s">
@@ -4760,35 +4792,29 @@
       <c r="I50" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="J50" s="3" t="s">
-        <v>374</v>
-      </c>
       <c r="L50" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q50" s="13" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="R50" s="13"/>
-      <c r="V50" s="1" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F51" s="12"/>
       <c r="G51" s="3" t="s">
@@ -4801,22 +4827,16 @@
         <v>29</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="L51" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q51" s="13" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="R51" s="13"/>
-      <c r="S51" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="T51" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="U51" s="1" t="s">
+      <c r="V51" s="1" t="s">
         <v>383</v>
       </c>
     </row>
@@ -4825,12 +4845,15 @@
         <v>384</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>385</v>
       </c>
       <c r="F52" s="12"/>
@@ -4844,39 +4867,36 @@
         <v>29</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="L52" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q52" s="13" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="R52" s="13"/>
       <c r="S52" s="1" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="T52" s="13" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="U52" s="1" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="E53" s="2" t="s">
         <v>392</v>
       </c>
       <c r="F53" s="12"/>
@@ -4890,7 +4910,7 @@
         <v>29</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>52</v>
+        <v>386</v>
       </c>
       <c r="L53" s="4" t="s">
         <v>84</v>
@@ -4899,25 +4919,28 @@
         <v>393</v>
       </c>
       <c r="R53" s="13"/>
+      <c r="S53" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="T53" s="13" t="s">
+        <v>395</v>
+      </c>
       <c r="U53" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="V53" s="1" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>399</v>
@@ -4930,7 +4953,10 @@
         <v>28</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>107</v>
+        <v>29</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="L54" s="4" t="s">
         <v>84</v>
@@ -4939,31 +4965,28 @@
         <v>400</v>
       </c>
       <c r="R54" s="13"/>
-      <c r="S54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="T54" s="13" t="s">
+      <c r="V54" s="1" t="s">
         <v>402</v>
-      </c>
-      <c r="U54" s="1" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>406</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>407</v>
       </c>
       <c r="F55" s="12"/>
       <c r="G55" s="3" t="s">
@@ -4975,46 +4998,38 @@
       <c r="I55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K55" s="4" t="s">
+      <c r="L55" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q55" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="R55" s="13"/>
+      <c r="S55" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="L55" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M55" s="4" t="s">
+      <c r="T55" s="13" t="s">
         <v>409</v>
       </c>
-      <c r="Q55" s="13" t="s">
+      <c r="U55" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="R55" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="S55" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="T55" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="U55" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>416</v>
+        <v>367</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F56" s="12"/>
       <c r="G56" s="3" t="s">
@@ -5024,28 +5039,39 @@
         <v>28</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>157</v>
+        <v>107</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>415</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>84</v>
+        <v>28</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>416</v>
       </c>
       <c r="Q56" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="S56" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="T56" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="R56" s="13"/>
-      <c r="T56" s="13" t="s">
+      <c r="U56" s="1" t="s">
         <v>421</v>
-      </c>
-      <c r="U56" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>424</v>
@@ -5066,43 +5092,37 @@
       <c r="I57" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J57" s="3" t="s">
-        <v>427</v>
-      </c>
       <c r="L57" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q57" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="R57" s="13"/>
+      <c r="T57" s="13" t="s">
         <v>428</v>
       </c>
-      <c r="R57" s="13"/>
-      <c r="S57" s="1" t="s">
+      <c r="U57" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="T57" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="U57" s="13"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="F58" s="12" t="s">
-        <v>435</v>
-      </c>
+      <c r="F58" s="12"/>
       <c r="G58" s="3" t="s">
         <v>51</v>
       </c>
@@ -5110,48 +5130,45 @@
         <v>28</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>436</v>
+        <v>157</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>434</v>
       </c>
       <c r="L58" s="4" t="s">
         <v>84</v>
       </c>
       <c r="Q58" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="R58" s="13"/>
       <c r="S58" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="T58" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="U58" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="V58" s="1" t="s">
-        <v>441</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="U58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F59" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="F59" s="12"/>
       <c r="G59" s="3" t="s">
         <v>51</v>
       </c>
@@ -5161,50 +5178,44 @@
       <c r="I59" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J59" s="3" t="s">
-        <v>270</v>
-      </c>
       <c r="K59" s="4" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M59" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="N59" s="5" t="s">
-        <v>447</v>
+        <v>84</v>
       </c>
       <c r="Q59" s="13" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="R59" s="13"/>
       <c r="S59" s="1" t="s">
-        <v>272</v>
+        <v>445</v>
       </c>
       <c r="T59" s="13" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
+      </c>
+      <c r="V59" s="1" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>453</v>
       </c>
       <c r="F60" s="12"/>
       <c r="G60" s="3" t="s">
@@ -5216,31 +5227,50 @@
       <c r="I60" s="3" t="s">
         <v>107</v>
       </c>
+      <c r="J60" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>453</v>
+      </c>
       <c r="L60" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M60" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="N60" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="V60" s="1" t="s">
+      <c r="Q60" s="13" t="s">
         <v>455</v>
+      </c>
+      <c r="R60" s="13"/>
+      <c r="S60" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="T60" s="13" t="s">
+        <v>456</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>458</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="F61" s="12"/>
       <c r="G61" s="3" t="s">
@@ -5253,49 +5283,34 @@
         <v>107</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M61" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="N61" s="5" t="s">
-        <v>447</v>
-      </c>
-      <c r="Q61" s="13" t="s">
-        <v>460</v>
-      </c>
-      <c r="S61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q61" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="T61" s="13" t="s">
+      <c r="V61" s="1" t="s">
         <v>462</v>
-      </c>
-      <c r="U61" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="V61" s="1" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>466</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>468</v>
       </c>
       <c r="F62" s="12"/>
       <c r="G62" s="3" t="s">
-        <v>469</v>
+        <v>51</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>28</v>
@@ -5307,54 +5322,58 @@
         <v>28</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q62" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="N62" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q62" s="13" t="s">
+        <v>467</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="T62" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="U62" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="S62" s="1" t="s">
+      <c r="V62" s="1" t="s">
         <v>471</v>
-      </c>
-      <c r="T62" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="U62" s="1" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>474</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>475</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="12"/>
+      <c r="G63" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="F63" s="18" t="n">
-        <v>45235</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="H63" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="N63" s="5" t="s">
-        <v>447</v>
+        <v>28</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="Q63" s="1" t="s">
         <v>477</v>
@@ -5367,6 +5386,53 @@
       </c>
       <c r="U63" s="1" t="s">
         <v>480</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="F64" s="18" t="n">
+        <v>45235</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="L64" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="U64" s="1" t="s">
+        <v>487</v>
       </c>
     </row>
   </sheetData>
@@ -5408,38 +5474,40 @@
     <hyperlink ref="T34" r:id="rId35" display="https://doi.org/10.1038/s41597-021-01006-6"/>
     <hyperlink ref="Q35" r:id="rId36" display="https://doi.org/10.6084/m9.figshare.c.3843841.v1"/>
     <hyperlink ref="T35" r:id="rId37" display="https://doi.org/10.1038/sdata.2018.135"/>
-    <hyperlink ref="Q36" r:id="rId38" display="https://www.idiv.de/de/splot.html"/>
-    <hyperlink ref="Q37" r:id="rId39" display="https://doi.org/10.25829/idiv.3474-40-3292"/>
-    <hyperlink ref="T37" r:id="rId40" display="https://doi.org/10.1111/geb.13346"/>
-    <hyperlink ref="Q38" r:id="rId41" display="https://lotvs.csic.es/"/>
-    <hyperlink ref="T38" r:id="rId42" display="https://www.biorxiv.org/content/10.1101/2021.09.29.462383v1.full"/>
-    <hyperlink ref="Q39" r:id="rId43" display="https://gfbinitiative.net/"/>
-    <hyperlink ref="Q40" r:id="rId44" display="http://icp-forests.net/"/>
-    <hyperlink ref="T41" r:id="rId45" display="https://doi.org/10.1016/j.srs.2020.100002"/>
-    <hyperlink ref="Q44" r:id="rId46" display="http://sapfluxnet.creaf.cat/"/>
-    <hyperlink ref="T44" r:id="rId47" display="https://doi.org/10.5194/essd-13-2607-2021"/>
-    <hyperlink ref="Q48" r:id="rId48" location="/home" display="https://data.isric.org/geonetwork/srv/eng/catalog.search#/home"/>
-    <hyperlink ref="T48" r:id="rId49" display="https://doi.org/10.5194/essd-9-1-2017"/>
-    <hyperlink ref="Q49" r:id="rId50" display="https://www.fao.org/soils-portal/data-hub/soil-maps-and-databases/harmonized-world-soil-database-v12/en/"/>
-    <hyperlink ref="Q50" r:id="rId51" display="https://soilgrids.org/"/>
-    <hyperlink ref="Q51" r:id="rId52" display="https://www.isric.org/explore/wise-databases"/>
-    <hyperlink ref="T51" r:id="rId53" display="https://doi.org/10.1016/j.geoderma.2016.01.034"/>
-    <hyperlink ref="Q52" r:id="rId54" display="http://globalchange.bnu.edu.cn/research/data"/>
-    <hyperlink ref="T52" r:id="rId55" display="http://doi.wiley.com/10.1002/2013MS000293"/>
-    <hyperlink ref="Q53" r:id="rId56" display="https://www.futurewater.eu/projects/hihydrosoil/"/>
-    <hyperlink ref="Q54" r:id="rId57" display="https://ismn.earth/en/"/>
-    <hyperlink ref="T54" r:id="rId58" display="https://doi.org/10.5194/hess-2021-2"/>
-    <hyperlink ref="Q55" r:id="rId59" display="https://doi.org/10.3334/ORNLDAAC/1827"/>
-    <hyperlink ref="T55" r:id="rId60" display="https://10.5194/bg-7-1915-2010"/>
-    <hyperlink ref="Q56" r:id="rId61" display="https://doi.pangaea.de/10.1594/PANGAEA.788537"/>
-    <hyperlink ref="T56" r:id="rId62" display="https://doi.org/10.1029/2012GC004370"/>
-    <hyperlink ref="Q57" r:id="rId63" display="https://dataverse.scholarsportal.info/dataset.xhtml"/>
-    <hyperlink ref="T57" r:id="rId64" display="https://doi.org/10.1002/2017GL075860"/>
-    <hyperlink ref="T58" r:id="rId65" display="https://doi.org/10.1016/j.cageo.2014.07.020"/>
-    <hyperlink ref="Q59" r:id="rId66" display="https://biotime.st-andrews.ac.uk/"/>
-    <hyperlink ref="T59" r:id="rId67" display="https://doi.org/10.1111/geb.12729"/>
-    <hyperlink ref="Q61" r:id="rId68" display="https://compadre-db.org/"/>
-    <hyperlink ref="T61" r:id="rId69" display="https://doi.org/10.1111/1365-2745.12334"/>
+    <hyperlink ref="Q36" r:id="rId38" display="https://doi.org/10.6084/m9.figshare.19448219.v6"/>
+    <hyperlink ref="T36" r:id="rId39" display="https://doi.org/10.1038/s41597-022-01884-4"/>
+    <hyperlink ref="Q37" r:id="rId40" display="https://www.idiv.de/de/splot.html"/>
+    <hyperlink ref="Q38" r:id="rId41" display="https://doi.org/10.25829/idiv.3474-40-3292"/>
+    <hyperlink ref="T38" r:id="rId42" display="https://doi.org/10.1111/geb.13346"/>
+    <hyperlink ref="Q39" r:id="rId43" display="https://lotvs.csic.es/"/>
+    <hyperlink ref="T39" r:id="rId44" display="https://www.biorxiv.org/content/10.1101/2021.09.29.462383v1.full"/>
+    <hyperlink ref="Q40" r:id="rId45" display="https://gfbinitiative.net/"/>
+    <hyperlink ref="Q41" r:id="rId46" display="http://icp-forests.net/"/>
+    <hyperlink ref="T42" r:id="rId47" display="https://doi.org/10.1016/j.srs.2020.100002"/>
+    <hyperlink ref="Q45" r:id="rId48" display="http://sapfluxnet.creaf.cat/"/>
+    <hyperlink ref="T45" r:id="rId49" display="https://doi.org/10.5194/essd-13-2607-2021"/>
+    <hyperlink ref="Q49" r:id="rId50" location="/home" display="https://data.isric.org/geonetwork/srv/eng/catalog.search#/home"/>
+    <hyperlink ref="T49" r:id="rId51" display="https://doi.org/10.5194/essd-9-1-2017"/>
+    <hyperlink ref="Q50" r:id="rId52" display="https://www.fao.org/soils-portal/data-hub/soil-maps-and-databases/harmonized-world-soil-database-v12/en/"/>
+    <hyperlink ref="Q51" r:id="rId53" display="https://soilgrids.org/"/>
+    <hyperlink ref="Q52" r:id="rId54" display="https://www.isric.org/explore/wise-databases"/>
+    <hyperlink ref="T52" r:id="rId55" display="https://doi.org/10.1016/j.geoderma.2016.01.034"/>
+    <hyperlink ref="Q53" r:id="rId56" display="http://globalchange.bnu.edu.cn/research/data"/>
+    <hyperlink ref="T53" r:id="rId57" display="http://doi.wiley.com/10.1002/2013MS000293"/>
+    <hyperlink ref="Q54" r:id="rId58" display="https://www.futurewater.eu/projects/hihydrosoil/"/>
+    <hyperlink ref="Q55" r:id="rId59" display="https://ismn.earth/en/"/>
+    <hyperlink ref="T55" r:id="rId60" display="https://doi.org/10.5194/hess-2021-2"/>
+    <hyperlink ref="Q56" r:id="rId61" display="https://doi.org/10.3334/ORNLDAAC/1827"/>
+    <hyperlink ref="T56" r:id="rId62" display="https://10.5194/bg-7-1915-2010"/>
+    <hyperlink ref="Q57" r:id="rId63" display="https://doi.pangaea.de/10.1594/PANGAEA.788537"/>
+    <hyperlink ref="T57" r:id="rId64" display="https://doi.org/10.1029/2012GC004370"/>
+    <hyperlink ref="Q58" r:id="rId65" display="https://dataverse.scholarsportal.info/dataset.xhtml"/>
+    <hyperlink ref="T58" r:id="rId66" display="https://doi.org/10.1002/2017GL075860"/>
+    <hyperlink ref="T59" r:id="rId67" display="https://doi.org/10.1016/j.cageo.2014.07.020"/>
+    <hyperlink ref="Q60" r:id="rId68" display="https://biotime.st-andrews.ac.uk/"/>
+    <hyperlink ref="T60" r:id="rId69" display="https://doi.org/10.1111/geb.12729"/>
+    <hyperlink ref="Q62" r:id="rId70" display="https://compadre-db.org/"/>
+    <hyperlink ref="T62" r:id="rId71" display="https://doi.org/10.1111/1365-2745.12334"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5462,22 +5530,22 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
external_data: updated GLHYMPS link
</commit_message>
<xml_diff>
--- a/ExternalDataSources.xlsx
+++ b/ExternalDataSources.xlsx
@@ -1973,7 +1973,7 @@
     <t xml:space="preserve">10 x 10 km (polygons)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://dataverse.scholarsportal.info/dataset.xhtml</t>
+    <t xml:space="preserve">https://borealisdata.ca/dataset.xhtml?persistentId=doi%3A10.5683/SP2/TTJNIU</t>
   </si>
   <si>
     <t xml:space="preserve">subsurface permeability, subsurface porosity</t>
@@ -2665,13 +2665,13 @@
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="G23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="G37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="Q63" activeCellId="0" sqref="Q63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="25.28"/>
@@ -5951,7 +5951,7 @@
     <hyperlink ref="Q61" r:id="rId69" display="https://icgc.cat/Administracio-i-empresa/Descarregues/Cartografia-geologica-i-geotematica/Cartografia-de-sols/Mapa-de-sols-1-25.000-continu"/>
     <hyperlink ref="Q62" r:id="rId70" display="https://doi.pangaea.de/10.1594/PANGAEA.788537"/>
     <hyperlink ref="T62" r:id="rId71" display="https://doi.org/10.1029/2012GC004370"/>
-    <hyperlink ref="Q63" r:id="rId72" display="https://dataverse.scholarsportal.info/dataset.xhtml"/>
+    <hyperlink ref="Q63" r:id="rId72" display="https://borealisdata.ca/dataset.xhtml?persistentId=doi%3A10.5683/SP2/TTJNIU"/>
     <hyperlink ref="T63" r:id="rId73" display="https://doi.org/10.1002/2017GL075860"/>
     <hyperlink ref="T64" r:id="rId74" display="https://doi.org/10.1016/j.cageo.2014.07.020"/>
     <hyperlink ref="Q65" r:id="rId75" display="https://biotime.st-andrews.ac.uk/"/>
@@ -5980,7 +5980,7 @@
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">

</xml_diff>